<commit_message>
Improve documentation and consistency in class methods
- Include cType.TaesLabPath function to determine dinamically the paths.
- Add new functions in Docs/Utilities to get class documentation
- Updated and expanded docstrings for many classes and methods to improve clarity and consistency, including corrections to method names, descriptions, and property lists.
- Fixed typos and standardized terminology across the codebase.
- Added or clarified usage syntax and output arguments in method documentation.
</commit_message>
<xml_diff>
--- a/Docs/Utilities/Contents.xlsx
+++ b/Docs/Utilities/Contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Docs\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F3D885-19EF-4FE9-8C8E-ADE805ED1FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ED6CE3-097A-4002-83B0-152BC2FB5973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="780" windowWidth="14520" windowHeight="14700" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="459">
   <si>
     <t>Name</t>
   </si>
@@ -675,12 +675,6 @@
     <t>Abstract class to read table data model.</t>
   </si>
   <si>
-    <t>%cReadModelXLS -Implement the cReadModelTable to read XLSX data model files</t>
-  </si>
-  <si>
-    <t>%cReadModelXML implements the cReadModelStruct to read XML data model files.</t>
-  </si>
-  <si>
     <t>Gets and validates the external cost resources of a productive structure.</t>
   </si>
   <si>
@@ -852,9 +846,6 @@
     <t>setRecycling</t>
   </si>
   <si>
-    <t>setRecycing - Set Recycling parameter</t>
-  </si>
-  <si>
     <t>setSummary</t>
   </si>
   <si>
@@ -960,9 +951,6 @@
     <t>isGeneralCost</t>
   </si>
   <si>
-    <t>isGeneralizedCost - Check if Generalized cost calculation are activated</t>
-  </si>
-  <si>
     <t>isResourceCost</t>
   </si>
   <si>
@@ -1074,9 +1062,6 @@
     <t>printResults</t>
   </si>
   <si>
-    <t>print the result tables on console</t>
-  </si>
-  <si>
     <t>saveResults</t>
   </si>
   <si>
@@ -1182,9 +1167,6 @@
     <t>setFlowResource</t>
   </si>
   <si>
-    <t>setFlowResources - Set the resource cost of the flows</t>
-  </si>
-  <si>
     <t>setProcessResource</t>
   </si>
   <si>
@@ -1209,9 +1191,6 @@
     <t>updateDataModel</t>
   </si>
   <si>
-    <t>update the data model if have been changes</t>
-  </si>
-  <si>
     <t>getResultState</t>
   </si>
   <si>
@@ -1410,10 +1389,25 @@
     <t>Thermoeconomic Model Methods</t>
   </si>
   <si>
-    <t>mt2td</t>
-  </si>
-  <si>
-    <t>Convert a MATLAB table into a cTableData object</t>
+    <t>Set Recycling parameter</t>
+  </si>
+  <si>
+    <t>Check if Generalized cost calculation are activated</t>
+  </si>
+  <si>
+    <t>Print the result tables on console</t>
+  </si>
+  <si>
+    <t>Set the resource cost of the flows</t>
+  </si>
+  <si>
+    <t>Update the data model if have been changes</t>
+  </si>
+  <si>
+    <t>Implement the cReadModelTable to read XLSX data model files</t>
+  </si>
+  <si>
+    <t>Implements the cReadModelStruct to read XML data model files.</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1737,41 +1731,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1808,14 +1767,16 @@
       <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1838,13 +1799,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2198,66 +2156,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="D1" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="D2" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C3" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D3" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C4" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D4" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B5" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C5" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="D5" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -2287,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2598,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,18 +2572,18 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="19">
@@ -2636,7 +2594,7 @@
       <c r="A3" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="15">
@@ -2647,7 +2605,7 @@
       <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>92</v>
       </c>
       <c r="C4" s="15">
@@ -2658,7 +2616,7 @@
       <c r="A5" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="24" t="s">
         <v>93</v>
       </c>
       <c r="C5" s="15">
@@ -2669,7 +2627,7 @@
       <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>94</v>
       </c>
       <c r="C6" s="15">
@@ -2680,7 +2638,7 @@
       <c r="A7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>95</v>
       </c>
       <c r="C7" s="15">
@@ -2691,7 +2649,7 @@
       <c r="A8" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="15">
@@ -2702,7 +2660,7 @@
       <c r="A9" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="24" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="15">
@@ -2713,7 +2671,7 @@
       <c r="A10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C10" s="15">
@@ -2724,7 +2682,7 @@
       <c r="A11" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="24" t="s">
         <v>99</v>
       </c>
       <c r="C11" s="15">
@@ -2735,7 +2693,7 @@
       <c r="A12" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C12" s="15">
@@ -2746,7 +2704,7 @@
       <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="24" t="s">
         <v>101</v>
       </c>
       <c r="C13" s="15">
@@ -2757,7 +2715,7 @@
       <c r="A14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="15">
@@ -2768,7 +2726,7 @@
       <c r="A15" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="24" t="s">
         <v>103</v>
       </c>
       <c r="C15" s="15">
@@ -2779,7 +2737,7 @@
       <c r="A16" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="24" t="s">
         <v>104</v>
       </c>
       <c r="C16" s="15">
@@ -2790,7 +2748,7 @@
       <c r="A17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="24" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="15">
@@ -2801,7 +2759,7 @@
       <c r="A18" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="24" t="s">
         <v>88</v>
       </c>
       <c r="C18" s="15">
@@ -2812,7 +2770,7 @@
       <c r="A19" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="24" t="s">
         <v>105</v>
       </c>
       <c r="C19" s="15">
@@ -2823,7 +2781,7 @@
       <c r="A20" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="24" t="s">
         <v>106</v>
       </c>
       <c r="C20" s="15">
@@ -2834,7 +2792,7 @@
       <c r="A21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="24" t="s">
         <v>107</v>
       </c>
       <c r="C21" s="15">
@@ -2845,7 +2803,7 @@
       <c r="A22" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="24" t="s">
         <v>108</v>
       </c>
       <c r="C22" s="15">
@@ -2856,7 +2814,7 @@
       <c r="A23" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="24" t="s">
         <v>109</v>
       </c>
       <c r="C23" s="15">
@@ -2867,7 +2825,7 @@
       <c r="A24" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="24" t="s">
         <v>110</v>
       </c>
       <c r="C24" s="15">
@@ -2878,7 +2836,7 @@
       <c r="A25" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="24" t="s">
         <v>111</v>
       </c>
       <c r="C25" s="15">
@@ -2889,7 +2847,7 @@
       <c r="A26" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="24" t="s">
         <v>112</v>
       </c>
       <c r="C26" s="15">
@@ -2900,7 +2858,7 @@
       <c r="A27" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="24" t="s">
         <v>113</v>
       </c>
       <c r="C27" s="15">
@@ -2911,7 +2869,7 @@
       <c r="A28" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="24" t="s">
         <v>114</v>
       </c>
       <c r="C28" s="15">
@@ -2922,7 +2880,7 @@
       <c r="A29" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="24" t="s">
         <v>115</v>
       </c>
       <c r="C29" s="15">
@@ -2933,7 +2891,7 @@
       <c r="A30" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="24" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="15">
@@ -2941,24 +2899,13 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>459</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>460</v>
-      </c>
-      <c r="C32" s="24">
+      <c r="C31" s="16">
         <v>4</v>
       </c>
     </row>
@@ -2975,8 +2922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2993,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3012,7 +2959,7 @@
         <v>171</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -3056,7 +3003,7 @@
         <v>173</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" s="17">
         <v>2</v>
@@ -3133,7 +3080,7 @@
         <v>153</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>214</v>
+        <v>457</v>
       </c>
       <c r="C14" s="17">
         <v>3</v>
@@ -3144,7 +3091,7 @@
         <v>154</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>215</v>
+        <v>458</v>
       </c>
       <c r="C15" s="17">
         <v>3</v>
@@ -3188,7 +3135,7 @@
         <v>155</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C19" s="17">
         <v>4</v>
@@ -3199,7 +3146,7 @@
         <v>159</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C20" s="17">
         <v>4</v>
@@ -3210,7 +3157,7 @@
         <v>176</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C21" s="17">
         <v>4</v>
@@ -3254,7 +3201,7 @@
         <v>156</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C25" s="17">
         <v>5</v>
@@ -3265,7 +3212,7 @@
         <v>157</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C26" s="17">
         <v>5</v>
@@ -3276,7 +3223,7 @@
         <v>158</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C27" s="17">
         <v>5</v>
@@ -3287,7 +3234,7 @@
         <v>172</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C28" s="17">
         <v>5</v>
@@ -3317,10 +3264,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C31" s="17">
         <v>6</v>
@@ -3328,10 +3275,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C32" s="17">
         <v>6</v>
@@ -3339,10 +3286,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C33" s="17">
         <v>6</v>
@@ -3350,10 +3297,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C34" s="17">
         <v>6</v>
@@ -3361,10 +3308,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C35" s="17">
         <v>6</v>
@@ -3372,10 +3319,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C36" s="17">
         <v>6</v>
@@ -3383,10 +3330,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C37" s="17">
         <v>6</v>
@@ -3394,21 +3341,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C38" s="17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C39" s="17">
         <v>7</v>
@@ -3416,10 +3363,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C40" s="17">
         <v>7</v>
@@ -3427,10 +3374,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C41" s="17">
         <v>7</v>
@@ -3438,10 +3385,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C42" s="17">
         <v>7</v>
@@ -3449,10 +3396,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C43" s="17">
         <v>7</v>
@@ -3460,10 +3407,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C44" s="17">
         <v>7</v>
@@ -3471,21 +3418,21 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="C45" s="17">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C46" s="17">
         <v>8</v>
@@ -3493,10 +3440,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C47" s="17">
         <v>8</v>
@@ -3504,10 +3451,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C48" s="17">
         <v>8</v>
@@ -3515,10 +3462,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="17">
         <v>8</v>
@@ -3526,10 +3473,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C50" s="17">
         <v>8</v>
@@ -3537,10 +3484,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C51" s="17">
         <v>8</v>
@@ -3548,10 +3495,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C52" s="17">
         <v>8</v>
@@ -3559,10 +3506,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C53" s="17">
         <v>8</v>
@@ -3570,21 +3517,21 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="C54" s="17">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C55" s="17">
         <v>9</v>
@@ -3592,10 +3539,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C56" s="17">
         <v>9</v>
@@ -3603,10 +3550,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>235</v>
+        <v>179</v>
       </c>
       <c r="C57" s="17">
         <v>9</v>
@@ -3614,21 +3561,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="C58" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C59" s="17">
         <v>10</v>
@@ -3661,7 +3608,7 @@
         <v>160</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C62" s="18">
         <v>10</v>
@@ -3680,8 +3627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E4B252-D3EB-4388-84A9-3E57780FCC8C}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3699,15 +3646,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3715,10 +3662,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3726,10 +3673,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3737,10 +3684,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3748,10 +3695,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3759,10 +3706,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3770,10 +3717,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>452</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3781,10 +3728,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3792,10 +3739,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3803,10 +3750,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3814,10 +3761,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -3825,10 +3772,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3836,10 +3783,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -3847,10 +3794,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3858,10 +3805,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B16" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3869,10 +3816,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B17" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -3880,10 +3827,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -3891,10 +3838,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B19" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3902,10 +3849,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3913,10 +3860,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -3924,10 +3871,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3935,10 +3882,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -3946,10 +3893,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3957,10 +3904,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B25" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -3968,10 +3915,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B26" t="s">
-        <v>309</v>
+        <v>453</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3979,10 +3926,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B27" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -3990,10 +3937,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -4001,10 +3948,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B29" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -4012,10 +3959,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B30" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -4023,10 +3970,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B31" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -4034,10 +3981,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B32" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -4045,10 +3992,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -4056,10 +4003,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B34" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -4067,10 +4014,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B35" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -4078,10 +4025,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -4089,10 +4036,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B37" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -4100,10 +4047,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B38" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -4111,10 +4058,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B39" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -4122,10 +4069,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B40" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -4133,10 +4080,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B41" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -4144,10 +4091,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B42" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -4155,10 +4102,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B43" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -4166,10 +4113,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B44" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -4177,10 +4124,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B45" t="s">
-        <v>347</v>
+        <v>454</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -4188,10 +4135,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B46" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -4199,10 +4146,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B47" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -4210,10 +4157,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B48" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C48">
         <v>6</v>
@@ -4221,10 +4168,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B49" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C49">
         <v>6</v>
@@ -4232,10 +4179,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B50" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C50">
         <v>6</v>
@@ -4243,10 +4190,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B51" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C51">
         <v>6</v>
@@ -4254,10 +4201,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B52" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C52">
         <v>6</v>
@@ -4265,10 +4212,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B53" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -4276,10 +4223,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B54" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -4287,10 +4234,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B55" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -4298,10 +4245,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B56" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -4309,10 +4256,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B57" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C57">
         <v>7</v>
@@ -4320,10 +4267,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B58" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -4331,10 +4278,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B59" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C59">
         <v>7</v>
@@ -4342,10 +4289,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B60" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C60">
         <v>7</v>
@@ -4353,10 +4300,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B61" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -4364,10 +4311,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B62" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -4375,10 +4322,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B63" t="s">
-        <v>383</v>
+        <v>455</v>
       </c>
       <c r="C63">
         <v>8</v>
@@ -4386,10 +4333,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B64" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C64">
         <v>8</v>
@@ -4397,10 +4344,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B65" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -4408,10 +4355,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B66" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C66">
         <v>9</v>
@@ -4419,10 +4366,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B67" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C67">
         <v>9</v>
@@ -4430,10 +4377,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B68" t="s">
-        <v>392</v>
+        <v>456</v>
       </c>
       <c r="C68">
         <v>10</v>
@@ -4441,10 +4388,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B69" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C69">
         <v>10</v>
@@ -4452,10 +4399,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B70" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C70">
         <v>10</v>
@@ -4463,10 +4410,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B71" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C71">
         <v>10</v>
@@ -4474,10 +4421,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="B72" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="C72">
         <v>10</v>
@@ -4485,10 +4432,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B73" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C73">
         <v>10</v>
@@ -4522,15 +4469,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4538,10 +4485,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4549,10 +4496,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4560,10 +4507,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4571,10 +4518,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4608,15 +4555,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B2" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4624,10 +4571,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4635,10 +4582,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4646,10 +4593,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4682,15 +4629,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4698,10 +4645,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4709,10 +4656,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4720,10 +4667,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4731,10 +4678,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4742,10 +4689,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -4753,10 +4700,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -4764,10 +4711,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -4775,10 +4722,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -4786,10 +4733,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -4823,15 +4770,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4839,10 +4786,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B3" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4850,10 +4797,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4861,10 +4808,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4872,10 +4819,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B6" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4883,10 +4830,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B7" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -4894,10 +4841,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B8" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -4905,10 +4852,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B9" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -4916,10 +4863,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B10" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -4927,10 +4874,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B11" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C11">
         <v>10</v>

</xml_diff>